<commit_message>
Average the activation function comparison over 10 passes
</commit_message>
<xml_diff>
--- a/activation_compare.xlsx
+++ b/activation_compare.xlsx
@@ -141,10 +141,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Arkusz1!$A$2:$A$101</c:f>
+              <c:f>Arkusz1!$A$2:$A$248</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="100"/>
+                <c:ptCount val="247"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -455,304 +455,304 @@
                 <c:formatCode>0.0000000000000000</c:formatCode>
                 <c:ptCount val="100"/>
                 <c:pt idx="0">
-                  <c:v>0.80554656418899995</c:v>
+                  <c:v>0.65947194656100006</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.69226545115899996</c:v>
+                  <c:v>0.63368161527300004</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.660297084737</c:v>
+                  <c:v>0.62270597113699999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.65000471683500005</c:v>
+                  <c:v>0.61442959582199996</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.64307635904100002</c:v>
+                  <c:v>0.60543843984000001</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.63663247824900004</c:v>
+                  <c:v>0.59519891140600001</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.63059367829599999</c:v>
+                  <c:v>0.58399509220099999</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.62479304118800005</c:v>
+                  <c:v>0.57231950356399997</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.61902781602500001</c:v>
+                  <c:v>0.560535090683</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.61310005560500003</c:v>
+                  <c:v>0.54889145580700005</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.60682556511499997</c:v>
+                  <c:v>0.53760175463000004</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.60003715774499999</c:v>
+                  <c:v>0.52684775526200001</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.59258562706399998</c:v>
+                  <c:v>0.51675156369999997</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.584342978869</c:v>
+                  <c:v>0.50736022685100002</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.57520928755599998</c:v>
+                  <c:v>0.498654893032</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.56512249692399996</c:v>
+                  <c:v>0.49057341268499999</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.55406936086299996</c:v>
+                  <c:v>0.48303302948499999</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.54209491010800004</c:v>
+                  <c:v>0.47594690035999998</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.52930736796800004</c:v>
+                  <c:v>0.46923411956099997</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.51587564524200002</c:v>
+                  <c:v>0.46282524002600001</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.50201775212800004</c:v>
+                  <c:v>0.45666542110699998</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.48798074040900002</c:v>
+                  <c:v>0.45071668720500002</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.474015572685</c:v>
+                  <c:v>0.44495992233300002</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.46035233357900002</c:v>
+                  <c:v>0.43939630430900001</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.44718119091500003</c:v>
+                  <c:v>0.43404705194999998</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.43464234108499999</c:v>
+                  <c:v>0.42894994915899998</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0.42282505152200001</c:v>
+                  <c:v>0.42415160992399997</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0.41177345467600002</c:v>
+                  <c:v>0.41969622508299997</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0.401495817561</c:v>
+                  <c:v>0.41561398603499999</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>0.39197443891700001</c:v>
+                  <c:v>0.41191344662599999</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>0.38317439705</c:v>
+                  <c:v>0.40858016935399999</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>0.37505042611700001</c:v>
+                  <c:v>0.40558056625799999</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>0.36755191067100002</c:v>
+                  <c:v>0.402867914868</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>0.36062632758300001</c:v>
+                  <c:v>0.400388029541</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>0.35422154198299999</c:v>
+                  <c:v>0.39808359997100001</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>0.34828730770499999</c:v>
+                  <c:v>0.39589736257500002</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>0.34277622508</c:v>
+                  <c:v>0.39377466878</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>0.33764432009299999</c:v>
+                  <c:v>0.3916658905</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>0.33285134729299998</c:v>
+                  <c:v>0.38952879157800002</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>0.32836088402500002</c:v>
+                  <c:v>0.38733076625599999</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>0.32414026699999998</c:v>
+                  <c:v>0.38505090367099998</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>0.32016041454700001</c:v>
+                  <c:v>0.38268221730700003</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>0.31639557288100001</c:v>
+                  <c:v>0.38023469558599998</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>0.31282301921599998</c:v>
+                  <c:v>0.37773921159200002</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>0.30942274818999999</c:v>
+                  <c:v>0.37525023906600002</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>0.306177161197</c:v>
+                  <c:v>0.37284313636499999</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>0.30307077191800003</c:v>
+                  <c:v>0.37060274704899998</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>0.30008993591100003</c:v>
+                  <c:v>0.36860550058500002</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>0.29722260804900003</c:v>
+                  <c:v>0.36690274290699998</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>0.294458128619</c:v>
+                  <c:v>0.36551283828100001</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>0.29178703707999998</c:v>
+                  <c:v>0.36442389196000002</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>0.28920091132300002</c:v>
+                  <c:v>0.36360332662599998</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>0.28669222982300002</c:v>
+                  <c:v>0.36300889088600002</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>0.28425425386399999</c:v>
+                  <c:v>0.362597361359</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>0.28188092716000002</c:v>
+                  <c:v>0.36232970639099998</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>0.27956679035699999</c:v>
+                  <c:v>0.36217316897700003</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>0.27730690822600002</c:v>
+                  <c:v>0.36210134279299999</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>0.27509680757900001</c:v>
+                  <c:v>0.362093260473</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>0.27293242428999998</c:v>
+                  <c:v>0.36213220678800001</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>0.27081005798699997</c:v>
+                  <c:v>0.36220464695600002</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>0.26872633324599998</c:v>
+                  <c:v>0.362299413919</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>0.26667816629300001</c:v>
+                  <c:v>0.36240714992799999</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>0.26466273638299997</c:v>
+                  <c:v>0.36251993618700001</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>0.26267746115500001</c:v>
+                  <c:v>0.36263104185799999</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>0.26071997537500002</c:v>
+                  <c:v>0.36273474814399997</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>0.25878811257200002</c:v>
+                  <c:v>0.36282622922300001</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>0.25687988912999998</c:v>
+                  <c:v>0.362901486941</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>0.25499349049499997</c:v>
+                  <c:v>0.36295733822300003</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>0.25312725915399997</c:v>
+                  <c:v>0.36299144724999999</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>0.251279684133</c:v>
+                  <c:v>0.36300238419800002</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>0.24944939177100001</c:v>
+                  <c:v>0.36298968409100002</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>0.247635137556</c:v>
+                  <c:v>0.36295387695199999</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>0.245835798844</c:v>
+                  <c:v>0.362896465532</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>0.24405036830599999</c:v>
+                  <c:v>0.362819838512</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>0.24227794795099999</c:v>
+                  <c:v>0.362727121815</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>0.24051774361100001</c:v>
+                  <c:v>0.36262198406399998</c:v>
                 </c:pt>
                 <c:pt idx="76">
-                  <c:v>0.238769059783</c:v>
+                  <c:v>0.36250842038199999</c:v>
                 </c:pt>
                 <c:pt idx="77">
-                  <c:v>0.23703129472500001</c:v>
+                  <c:v>0.36239054000400001</c:v>
                 </c:pt>
                 <c:pt idx="78">
-                  <c:v>0.235303935746</c:v>
+                  <c:v>0.36227237825300002</c:v>
                 </c:pt>
                 <c:pt idx="79">
-                  <c:v>0.233586554606</c:v>
+                  <c:v>0.36215774507499998</c:v>
                 </c:pt>
                 <c:pt idx="80">
-                  <c:v>0.23187880298300001</c:v>
+                  <c:v>0.362050113349</c:v>
                 </c:pt>
                 <c:pt idx="81">
-                  <c:v>0.23018040796799999</c:v>
+                  <c:v>0.361952542923</c:v>
                 </c:pt>
                 <c:pt idx="82">
-                  <c:v>0.22849116753900001</c:v>
+                  <c:v>0.36186763186100002</c:v>
                 </c:pt>
                 <c:pt idx="83">
-                  <c:v>0.22681094600500001</c:v>
+                  <c:v>0.36179748461599998</c:v>
                 </c:pt>
                 <c:pt idx="84">
-                  <c:v>0.22513966939800001</c:v>
+                  <c:v>0.36174368733099999</c:v>
                 </c:pt>
                 <c:pt idx="85">
-                  <c:v>0.223477320796</c:v>
+                  <c:v>0.36170728240400002</c:v>
                 </c:pt>
                 <c:pt idx="86">
-                  <c:v>0.221823935597</c:v>
+                  <c:v>0.36168873740500002</c:v>
                 </c:pt>
                 <c:pt idx="87">
-                  <c:v>0.220179596723</c:v>
+                  <c:v>0.36168790719100002</c:v>
                 </c:pt>
                 <c:pt idx="88">
-                  <c:v>0.21854442977999999</c:v>
+                  <c:v>0.36170399260800001</c:v>
                 </c:pt>
                 <c:pt idx="89">
-                  <c:v>0.21691859818199999</c:v>
+                  <c:v>0.36173550455499998</c:v>
                 </c:pt>
                 <c:pt idx="90">
-                  <c:v>0.21530229826200001</c:v>
+                  <c:v>0.36178024801199998</c:v>
                 </c:pt>
                 <c:pt idx="91">
-                  <c:v>0.21369575439399999</c:v>
+                  <c:v>0.36183534563800002</c:v>
                 </c:pt>
                 <c:pt idx="92">
-                  <c:v>0.21209921413899999</c:v>
+                  <c:v>0.36189732230400001</c:v>
                 </c:pt>
                 <c:pt idx="93">
-                  <c:v>0.210512943471</c:v>
+                  <c:v>0.36196226725199998</c:v>
                 </c:pt>
                 <c:pt idx="94">
-                  <c:v>0.20893722209099999</c:v>
+                  <c:v>0.36202607693700001</c:v>
                 </c:pt>
                 <c:pt idx="95">
-                  <c:v>0.20737233887100001</c:v>
+                  <c:v>0.36208476022899999</c:v>
                 </c:pt>
                 <c:pt idx="96">
-                  <c:v>0.20581858747599999</c:v>
+                  <c:v>0.36213476522799998</c:v>
                 </c:pt>
                 <c:pt idx="97">
-                  <c:v>0.20427626218</c:v>
+                  <c:v>0.362173274032</c:v>
                 </c:pt>
                 <c:pt idx="98">
-                  <c:v>0.20274565392800001</c:v>
+                  <c:v>0.362198416977</c:v>
                 </c:pt>
                 <c:pt idx="99">
-                  <c:v>0.20122704667399999</c:v>
+                  <c:v>0.36220938022900001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -778,10 +778,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Arkusz1!$A$2:$A$101</c:f>
+              <c:f>Arkusz1!$A$2:$A$248</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="100"/>
+                <c:ptCount val="247"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -1092,304 +1092,304 @@
                 <c:formatCode>0.0000000000000000</c:formatCode>
                 <c:ptCount val="100"/>
                 <c:pt idx="0">
-                  <c:v>0.327509347916</c:v>
+                  <c:v>0.31944784083200001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.32512465443999999</c:v>
+                  <c:v>0.30433127225899997</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.35083475871899999</c:v>
+                  <c:v>0.23491976833799999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.35060611427600002</c:v>
+                  <c:v>0.19432551066000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.34675987561100002</c:v>
+                  <c:v>0.179895982348</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.33329889782099997</c:v>
+                  <c:v>0.168168848195</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.29657719546400002</c:v>
+                  <c:v>0.161934221554</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.24773607393399999</c:v>
+                  <c:v>0.15841472242400001</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.21274520740700001</c:v>
+                  <c:v>0.151824036399</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.192089435808</c:v>
+                  <c:v>0.14410997401199999</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.17975253370899999</c:v>
+                  <c:v>0.137045335687</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.16576294932300001</c:v>
+                  <c:v>0.12794835822699999</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.152560898449</c:v>
+                  <c:v>0.116373542883</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.14276450164900001</c:v>
+                  <c:v>0.11129558170000001</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.13722178140999999</c:v>
+                  <c:v>0.106973366206</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.13414221787300001</c:v>
+                  <c:v>0.101503148852</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.13182593228700001</c:v>
+                  <c:v>9.5964512714600006E-2</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.130199707548</c:v>
+                  <c:v>9.1750288430099997E-2</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.12867145468899999</c:v>
+                  <c:v>8.8718132032400004E-2</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.12720769858</c:v>
+                  <c:v>8.6073629473699995E-2</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.12561678097500001</c:v>
+                  <c:v>8.3462615947600002E-2</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.123823669104</c:v>
+                  <c:v>8.0729818398299999E-2</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.121799617458</c:v>
+                  <c:v>7.7802491255200001E-2</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.119660607658</c:v>
+                  <c:v>7.4679692994100003E-2</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.117595314943</c:v>
+                  <c:v>7.1398980069599993E-2</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.11559621434</c:v>
+                  <c:v>6.7959761025399995E-2</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0.11358939204100001</c:v>
+                  <c:v>6.4301805693799993E-2</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0.111595804634</c:v>
+                  <c:v>6.0288487501500003E-2</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0.109647471545</c:v>
+                  <c:v>5.5914613666500003E-2</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>0.107754579287</c:v>
+                  <c:v>5.1450614983999998E-2</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>0.105922650942</c:v>
+                  <c:v>4.70943851161E-2</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>0.10414955767300001</c:v>
+                  <c:v>4.28695964193E-2</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>0.10241697924</c:v>
+                  <c:v>3.8857454205000003E-2</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>0.10069378842899999</c:v>
+                  <c:v>3.5127290172400003E-2</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>9.8943523955699997E-2</c:v>
+                  <c:v>3.1818789877E-2</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>9.7126047424600001E-2</c:v>
+                  <c:v>2.90424844067E-2</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>9.5193099818800003E-2</c:v>
+                  <c:v>2.6859754262300001E-2</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>9.3082629322600002E-2</c:v>
+                  <c:v>2.5217640154399999E-2</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>9.0717056656200001E-2</c:v>
+                  <c:v>2.4015571732700001E-2</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>8.8010692277999999E-2</c:v>
+                  <c:v>2.3169240174599998E-2</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>8.4883776039000006E-2</c:v>
+                  <c:v>2.2593303725599999E-2</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>8.1247012098599997E-2</c:v>
+                  <c:v>2.2205401376600001E-2</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>7.6918161240000005E-2</c:v>
+                  <c:v>2.1941625630699998E-2</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>7.1605799203100007E-2</c:v>
+                  <c:v>2.1759903959500001E-2</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>6.5204150287799995E-2</c:v>
+                  <c:v>2.1634265235200002E-2</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>5.7874361433600002E-2</c:v>
+                  <c:v>2.1548457814799998E-2</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>4.9593286397200002E-2</c:v>
+                  <c:v>2.1491815836199999E-2</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>4.1165995102499998E-2</c:v>
+                  <c:v>2.14569952578E-2</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>3.4467093487500003E-2</c:v>
+                  <c:v>2.1438749524999998E-2</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>3.0005858591099999E-2</c:v>
+                  <c:v>2.14332278582E-2</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>2.7038464221400001E-2</c:v>
+                  <c:v>2.14375443265E-2</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>2.4973953981499999E-2</c:v>
+                  <c:v>2.1449498881E-2</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>2.3571324211399999E-2</c:v>
+                  <c:v>2.14673902336E-2</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>2.26397190336E-2</c:v>
+                  <c:v>2.1489887111999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>2.2017737006500001E-2</c:v>
+                  <c:v>2.1515937786799999E-2</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>2.1596370221299999E-2</c:v>
+                  <c:v>2.1544705219699999E-2</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>2.1310446786300001E-2</c:v>
+                  <c:v>2.1575519661399999E-2</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>2.1120581327900002E-2</c:v>
+                  <c:v>2.1607843327700001E-2</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>2.10011047757E-2</c:v>
+                  <c:v>2.1641243584600001E-2</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>2.0934099386999999E-2</c:v>
+                  <c:v>2.1675372240200001E-2</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>2.0906535477499998E-2</c:v>
+                  <c:v>2.1709949307200001E-2</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>2.0908724349299999E-2</c:v>
+                  <c:v>2.1744750105800001E-2</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>2.09333618808E-2</c:v>
+                  <c:v>2.1779594913200001E-2</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>2.0974885914799998E-2</c:v>
+                  <c:v>2.18143405912E-2</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>2.10290264754E-2</c:v>
+                  <c:v>2.1848873776200001E-2</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>2.1092484072300001E-2</c:v>
+                  <c:v>2.18831053214E-2</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>2.1162696145999998E-2</c:v>
+                  <c:v>2.1916965751900001E-2</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>2.1237665285300002E-2</c:v>
+                  <c:v>2.1950401547600001E-2</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>2.13158313143E-2</c:v>
+                  <c:v>2.19833721047E-2</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>2.1395974911399999E-2</c:v>
+                  <c:v>2.2015847255700001E-2</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>2.14771441706E-2</c:v>
+                  <c:v>2.2047805249100001E-2</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>2.1558598066099999E-2</c:v>
+                  <c:v>2.20792311074E-2</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>2.16397625265E-2</c:v>
+                  <c:v>2.2110115296600001E-2</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>2.17201960322E-2</c:v>
+                  <c:v>2.21404526499E-2</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>2.1799562488799998E-2</c:v>
+                  <c:v>2.2170241500399999E-2</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>2.1877609720799999E-2</c:v>
+                  <c:v>2.21994829835E-2</c:v>
                 </c:pt>
                 <c:pt idx="76">
-                  <c:v>2.1954152345800001E-2</c:v>
+                  <c:v>2.2228180477700001E-2</c:v>
                 </c:pt>
                 <c:pt idx="77">
-                  <c:v>2.20290580935E-2</c:v>
+                  <c:v>2.2256339157399999E-2</c:v>
                 </c:pt>
                 <c:pt idx="78">
-                  <c:v>2.2102236849799999E-2</c:v>
+                  <c:v>2.2283965636099998E-2</c:v>
                 </c:pt>
                 <c:pt idx="79">
-                  <c:v>2.2173631870100002E-2</c:v>
+                  <c:v>2.2311067683100001E-2</c:v>
                 </c:pt>
                 <c:pt idx="80">
-                  <c:v>2.2243212726100001E-2</c:v>
+                  <c:v>2.2337653998100001E-2</c:v>
                 </c:pt>
                 <c:pt idx="81">
-                  <c:v>2.2310969641199999E-2</c:v>
+                  <c:v>2.2363734033300001E-2</c:v>
                 </c:pt>
                 <c:pt idx="82">
-                  <c:v>2.2376908942E-2</c:v>
+                  <c:v>2.2389317851800001E-2</c:v>
                 </c:pt>
                 <c:pt idx="83">
-                  <c:v>2.2441049407200001E-2</c:v>
+                  <c:v>2.2414416017000002E-2</c:v>
                 </c:pt>
                 <c:pt idx="84">
-                  <c:v>2.2503419339600001E-2</c:v>
+                  <c:v>2.2439039503799999E-2</c:v>
                 </c:pt>
                 <c:pt idx="85">
-                  <c:v>2.2564054219900001E-2</c:v>
+                  <c:v>2.2463199628800001E-2</c:v>
                 </c:pt>
                 <c:pt idx="86">
-                  <c:v>2.26229948296E-2</c:v>
+                  <c:v>2.24869079943E-2</c:v>
                 </c:pt>
                 <c:pt idx="87">
-                  <c:v>2.2680285751799999E-2</c:v>
+                  <c:v>2.2510176442099999E-2</c:v>
                 </c:pt>
                 <c:pt idx="88">
-                  <c:v>2.2735974175899999E-2</c:v>
+                  <c:v>2.2533017016500002E-2</c:v>
                 </c:pt>
                 <c:pt idx="89">
-                  <c:v>2.2790108947900001E-2</c:v>
+                  <c:v>2.2555441931600001E-2</c:v>
                 </c:pt>
                 <c:pt idx="90">
-                  <c:v>2.2842739817599999E-2</c:v>
+                  <c:v>2.2577463542799998E-2</c:v>
                 </c:pt>
                 <c:pt idx="91">
-                  <c:v>2.2893916844900001E-2</c:v>
+                  <c:v>2.2599094320900001E-2</c:v>
                 </c:pt>
                 <c:pt idx="92">
-                  <c:v>2.2943689933499999E-2</c:v>
+                  <c:v>2.26203468262E-2</c:v>
                 </c:pt>
                 <c:pt idx="93">
-                  <c:v>2.29921084683E-2</c:v>
+                  <c:v>2.26412336837E-2</c:v>
                 </c:pt>
                 <c:pt idx="94">
-                  <c:v>2.3039221035100001E-2</c:v>
+                  <c:v>2.26617675574E-2</c:v>
                 </c:pt>
                 <c:pt idx="95">
-                  <c:v>2.3085075206600001E-2</c:v>
+                  <c:v>2.2681961123E-2</c:v>
                 </c:pt>
                 <c:pt idx="96">
-                  <c:v>2.3129717382900001E-2</c:v>
+                  <c:v>2.2701827039200002E-2</c:v>
                 </c:pt>
                 <c:pt idx="97">
-                  <c:v>2.3173192674E-2</c:v>
+                  <c:v>2.2721377918E-2</c:v>
                 </c:pt>
                 <c:pt idx="98">
-                  <c:v>2.3215544817999999E-2</c:v>
+                  <c:v>2.27406262922E-2</c:v>
                 </c:pt>
                 <c:pt idx="99">
-                  <c:v>2.3256816125899998E-2</c:v>
+                  <c:v>2.2759584582499999E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1415,10 +1415,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Arkusz1!$A$2:$A$101</c:f>
+              <c:f>Arkusz1!$A$2:$A$248</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="100"/>
+                <c:ptCount val="247"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -1729,304 +1729,304 @@
                 <c:formatCode>0.0000000000000000</c:formatCode>
                 <c:ptCount val="100"/>
                 <c:pt idx="0">
-                  <c:v>0.49854756702500003</c:v>
+                  <c:v>0.170345875461</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.35136520545</c:v>
+                  <c:v>0.18903064973</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.30959201214100002</c:v>
+                  <c:v>0.13763419792699999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.28914039576700001</c:v>
+                  <c:v>0.108135490183</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.28860203688399999</c:v>
+                  <c:v>8.3234594508900001E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.20253121991799999</c:v>
+                  <c:v>7.1316306023000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.17125226309399999</c:v>
+                  <c:v>6.6316592487500006E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.15410377669</c:v>
+                  <c:v>6.2344106905499998E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.141840668753</c:v>
+                  <c:v>6.0283885746599999E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.14195119304699999</c:v>
+                  <c:v>5.8538086400699997E-2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.14270036089400001</c:v>
+                  <c:v>5.5965265165999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.14308701596199999</c:v>
+                  <c:v>5.4510837537599999E-2</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.143103312402</c:v>
+                  <c:v>5.3124856982999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.141834824271</c:v>
+                  <c:v>5.2068626769899998E-2</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.13259396091600001</c:v>
+                  <c:v>5.1093446985199999E-2</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.12219337072</c:v>
+                  <c:v>5.0248456620700002E-2</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.107234478429</c:v>
+                  <c:v>4.9479246746299999E-2</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.100113052467</c:v>
+                  <c:v>4.8692161844E-2</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>9.01149922825E-2</c:v>
+                  <c:v>4.7755079942799997E-2</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>7.4069564636899995E-2</c:v>
+                  <c:v>4.7242679311700002E-2</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>6.4198415500899997E-2</c:v>
+                  <c:v>4.6899102053100002E-2</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>5.9101535604900002E-2</c:v>
+                  <c:v>4.6530683822700002E-2</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>5.64756064452E-2</c:v>
+                  <c:v>4.6138414098100003E-2</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>5.3690001017599999E-2</c:v>
+                  <c:v>4.3996111176400003E-2</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>5.19292441031E-2</c:v>
+                  <c:v>4.3475248324299998E-2</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>5.09234287737E-2</c:v>
+                  <c:v>4.3523584376500002E-2</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>5.0373168388200003E-2</c:v>
+                  <c:v>4.3074911228899997E-2</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>4.9753958882099998E-2</c:v>
+                  <c:v>4.2882167797599999E-2</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>4.9203150638200001E-2</c:v>
+                  <c:v>4.2695712945900001E-2</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>4.8543402866799999E-2</c:v>
+                  <c:v>4.2620310498199997E-2</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>4.81220011229E-2</c:v>
+                  <c:v>4.25925449754E-2</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>4.7863176803900002E-2</c:v>
+                  <c:v>4.2601950229199999E-2</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>4.7640836945099997E-2</c:v>
+                  <c:v>4.25672831574E-2</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>4.7519556104299997E-2</c:v>
+                  <c:v>4.2650869346999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>4.7463555423700003E-2</c:v>
+                  <c:v>4.2425738542100001E-2</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>4.7460679022799997E-2</c:v>
+                  <c:v>4.2540524281100001E-2</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>4.7501966045299999E-2</c:v>
+                  <c:v>4.2772117213500001E-2</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>4.7584196629500003E-2</c:v>
+                  <c:v>4.2810427904300001E-2</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>4.76953547327E-2</c:v>
+                  <c:v>4.3084639327300001E-2</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>4.7795787405199998E-2</c:v>
+                  <c:v>4.3244048616699997E-2</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>4.7814139870299997E-2</c:v>
+                  <c:v>4.3454181567400003E-2</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>4.7848748347400001E-2</c:v>
+                  <c:v>4.3692220748300002E-2</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>4.78945102053E-2</c:v>
+                  <c:v>4.39600148658E-2</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>4.7954160287200003E-2</c:v>
+                  <c:v>4.4245495465100003E-2</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>4.8023220426300001E-2</c:v>
+                  <c:v>4.4649663821299999E-2</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>4.81002348336E-2</c:v>
+                  <c:v>4.4959466251800001E-2</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>4.81837747353E-2</c:v>
+                  <c:v>4.6418392431400002E-2</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>4.8272751324099999E-2</c:v>
+                  <c:v>4.6288951984000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>4.8369052414400003E-2</c:v>
+                  <c:v>4.6588506521699997E-2</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>4.8470281059600002E-2</c:v>
+                  <c:v>4.6297848248500001E-2</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>4.8575322621100002E-2</c:v>
+                  <c:v>4.5864488155099997E-2</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>4.86835134847E-2</c:v>
+                  <c:v>4.5556539480700001E-2</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>4.8794398427999999E-2</c:v>
+                  <c:v>4.4384468582100003E-2</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>4.8907948989999998E-2</c:v>
+                  <c:v>4.3796630452400002E-2</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>4.90239045453E-2</c:v>
+                  <c:v>4.2981783443799999E-2</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>4.9142004133699999E-2</c:v>
+                  <c:v>4.3063526743799999E-2</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>4.9262170637600002E-2</c:v>
+                  <c:v>4.3533137537300003E-2</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>4.9384254518900002E-2</c:v>
+                  <c:v>4.3921066230500003E-2</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>4.9507929431399998E-2</c:v>
+                  <c:v>4.38532449757E-2</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>4.9633062866399999E-2</c:v>
+                  <c:v>4.3982965858600002E-2</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>4.9759441393499998E-2</c:v>
+                  <c:v>4.4282772808900001E-2</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>4.98874692983E-2</c:v>
+                  <c:v>4.4571298768300002E-2</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>5.0018070377300002E-2</c:v>
+                  <c:v>4.51914881905E-2</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>5.0150660637499997E-2</c:v>
+                  <c:v>4.5990516251099997E-2</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>5.0284370980999998E-2</c:v>
+                  <c:v>4.7840880006299998E-2</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>5.0419133466E-2</c:v>
+                  <c:v>5.3609877573699997E-2</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>5.05549354829E-2</c:v>
+                  <c:v>5.1632260236699999E-2</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>5.0691777952E-2</c:v>
+                  <c:v>5.6203491671999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>5.0829666856899998E-2</c:v>
+                  <c:v>5.85175214463E-2</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>5.0968611202199997E-2</c:v>
+                  <c:v>5.6247856064100002E-2</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>5.11086222681E-2</c:v>
+                  <c:v>5.1976224754000003E-2</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>5.1249713139299997E-2</c:v>
+                  <c:v>4.8662203624199998E-2</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>5.1391898321800002E-2</c:v>
+                  <c:v>4.4849812917199999E-2</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>5.1535193407800002E-2</c:v>
+                  <c:v>4.3098904660100003E-2</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>5.16796147727E-2</c:v>
+                  <c:v>4.0137199697599997E-2</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>5.1822394371699998E-2</c:v>
+                  <c:v>3.6432823618499997E-2</c:v>
                 </c:pt>
                 <c:pt idx="76">
-                  <c:v>5.1967988956099997E-2</c:v>
+                  <c:v>3.3997328561899999E-2</c:v>
                 </c:pt>
                 <c:pt idx="77">
-                  <c:v>5.2115461104999997E-2</c:v>
+                  <c:v>3.3093329802100002E-2</c:v>
                 </c:pt>
                 <c:pt idx="78">
-                  <c:v>5.2264399814699998E-2</c:v>
+                  <c:v>3.0939244933300001E-2</c:v>
                 </c:pt>
                 <c:pt idx="79">
-                  <c:v>5.2414885129900002E-2</c:v>
+                  <c:v>3.0386018166399999E-2</c:v>
                 </c:pt>
                 <c:pt idx="80">
-                  <c:v>5.25668706024E-2</c:v>
+                  <c:v>2.9868952767399998E-2</c:v>
                 </c:pt>
                 <c:pt idx="81">
-                  <c:v>5.27203497735E-2</c:v>
+                  <c:v>2.8729823774200001E-2</c:v>
                 </c:pt>
                 <c:pt idx="82">
-                  <c:v>5.2875320461500001E-2</c:v>
+                  <c:v>2.8339435015100001E-2</c:v>
                 </c:pt>
                 <c:pt idx="83">
-                  <c:v>5.3028388429100001E-2</c:v>
+                  <c:v>2.81387112901E-2</c:v>
                 </c:pt>
                 <c:pt idx="84">
-                  <c:v>5.3181567957199999E-2</c:v>
+                  <c:v>2.79099234092E-2</c:v>
                 </c:pt>
                 <c:pt idx="85">
-                  <c:v>5.3336140089700002E-2</c:v>
+                  <c:v>2.7885086546300002E-2</c:v>
                 </c:pt>
                 <c:pt idx="86">
-                  <c:v>5.3492005073899999E-2</c:v>
+                  <c:v>2.7746583176200001E-2</c:v>
                 </c:pt>
                 <c:pt idx="87">
-                  <c:v>5.3649153715499998E-2</c:v>
+                  <c:v>2.7706075258599999E-2</c:v>
                 </c:pt>
                 <c:pt idx="88">
-                  <c:v>5.3807600006499999E-2</c:v>
+                  <c:v>2.7516317019700001E-2</c:v>
                 </c:pt>
                 <c:pt idx="89">
-                  <c:v>5.3967354040199998E-2</c:v>
+                  <c:v>2.7400943541199999E-2</c:v>
                 </c:pt>
                 <c:pt idx="90">
-                  <c:v>5.4128421151799999E-2</c:v>
+                  <c:v>2.71895343994E-2</c:v>
                 </c:pt>
                 <c:pt idx="91">
-                  <c:v>5.42662039161E-2</c:v>
+                  <c:v>2.7119308096500001E-2</c:v>
                 </c:pt>
                 <c:pt idx="92">
-                  <c:v>5.4378228759800001E-2</c:v>
+                  <c:v>2.6935047878399999E-2</c:v>
                 </c:pt>
                 <c:pt idx="93">
-                  <c:v>5.4483131708899998E-2</c:v>
+                  <c:v>2.67823531554E-2</c:v>
                 </c:pt>
                 <c:pt idx="94">
-                  <c:v>5.4590277609099999E-2</c:v>
+                  <c:v>2.6644454832200001E-2</c:v>
                 </c:pt>
                 <c:pt idx="95">
-                  <c:v>5.47008582592E-2</c:v>
+                  <c:v>2.6580612120499999E-2</c:v>
                 </c:pt>
                 <c:pt idx="96">
-                  <c:v>5.48136230869E-2</c:v>
+                  <c:v>2.6446171996099999E-2</c:v>
                 </c:pt>
                 <c:pt idx="97">
-                  <c:v>5.4928493055100003E-2</c:v>
+                  <c:v>2.6332486613E-2</c:v>
                 </c:pt>
                 <c:pt idx="98">
-                  <c:v>5.5045523079100003E-2</c:v>
+                  <c:v>2.6241760678099999E-2</c:v>
                 </c:pt>
                 <c:pt idx="99">
-                  <c:v>5.5164807540199999E-2</c:v>
+                  <c:v>2.6326490967300002E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2041,11 +2041,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="67865408"/>
-        <c:axId val="67865984"/>
+        <c:axId val="103815360"/>
+        <c:axId val="103815936"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="67865408"/>
+        <c:axId val="103815360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -2076,16 +2076,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="67865984"/>
+        <c:crossAx val="103815936"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
-        <c:majorUnit val="10"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="67865984"/>
+        <c:axId val="103815936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="1"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -2118,7 +2116,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="67865408"/>
+        <c:crossAx val="103815360"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2155,13 +2153,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>257175</xdr:colOff>
-      <xdr:row>55</xdr:row>
-      <xdr:rowOff>185736</xdr:rowOff>
+      <xdr:colOff>257174</xdr:colOff>
+      <xdr:row>64</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>25</xdr:col>
-      <xdr:colOff>295275</xdr:colOff>
+      <xdr:colOff>228599</xdr:colOff>
       <xdr:row>99</xdr:row>
       <xdr:rowOff>133349</xdr:rowOff>
     </xdr:to>
@@ -2476,10 +2474,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D105"/>
+  <dimension ref="A1:D248"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="F105" sqref="F105"/>
+    <sheetView tabSelected="1" topLeftCell="A62" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C254" sqref="C254"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2504,13 +2502,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="3">
-        <v>0.80554656418899995</v>
+        <v>0.65947194656100006</v>
       </c>
       <c r="C2" s="3">
-        <v>0.327509347916</v>
+        <v>0.31944784083200001</v>
       </c>
       <c r="D2" s="3">
-        <v>0.49854756702500003</v>
+        <v>0.170345875461</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -2518,13 +2516,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="3">
-        <v>0.69226545115899996</v>
+        <v>0.63368161527300004</v>
       </c>
       <c r="C3" s="3">
-        <v>0.32512465443999999</v>
+        <v>0.30433127225899997</v>
       </c>
       <c r="D3" s="3">
-        <v>0.35136520545</v>
+        <v>0.18903064973</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -2532,13 +2530,13 @@
         <v>3</v>
       </c>
       <c r="B4" s="3">
-        <v>0.660297084737</v>
+        <v>0.62270597113699999</v>
       </c>
       <c r="C4" s="3">
-        <v>0.35083475871899999</v>
+        <v>0.23491976833799999</v>
       </c>
       <c r="D4" s="3">
-        <v>0.30959201214100002</v>
+        <v>0.13763419792699999</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -2546,13 +2544,13 @@
         <v>4</v>
       </c>
       <c r="B5" s="3">
-        <v>0.65000471683500005</v>
+        <v>0.61442959582199996</v>
       </c>
       <c r="C5" s="3">
-        <v>0.35060611427600002</v>
+        <v>0.19432551066000001</v>
       </c>
       <c r="D5" s="3">
-        <v>0.28914039576700001</v>
+        <v>0.108135490183</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -2560,13 +2558,13 @@
         <v>5</v>
       </c>
       <c r="B6" s="3">
-        <v>0.64307635904100002</v>
+        <v>0.60543843984000001</v>
       </c>
       <c r="C6" s="3">
-        <v>0.34675987561100002</v>
+        <v>0.179895982348</v>
       </c>
       <c r="D6" s="3">
-        <v>0.28860203688399999</v>
+        <v>8.3234594508900001E-2</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -2574,13 +2572,13 @@
         <v>6</v>
       </c>
       <c r="B7" s="3">
-        <v>0.63663247824900004</v>
+        <v>0.59519891140600001</v>
       </c>
       <c r="C7" s="3">
-        <v>0.33329889782099997</v>
+        <v>0.168168848195</v>
       </c>
       <c r="D7" s="3">
-        <v>0.20253121991799999</v>
+        <v>7.1316306023000001E-2</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -2588,13 +2586,13 @@
         <v>7</v>
       </c>
       <c r="B8" s="3">
-        <v>0.63059367829599999</v>
+        <v>0.58399509220099999</v>
       </c>
       <c r="C8" s="3">
-        <v>0.29657719546400002</v>
+        <v>0.161934221554</v>
       </c>
       <c r="D8" s="3">
-        <v>0.17125226309399999</v>
+        <v>6.6316592487500006E-2</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -2602,13 +2600,13 @@
         <v>8</v>
       </c>
       <c r="B9" s="3">
-        <v>0.62479304118800005</v>
+        <v>0.57231950356399997</v>
       </c>
       <c r="C9" s="3">
-        <v>0.24773607393399999</v>
+        <v>0.15841472242400001</v>
       </c>
       <c r="D9" s="3">
-        <v>0.15410377669</v>
+        <v>6.2344106905499998E-2</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -2616,13 +2614,13 @@
         <v>9</v>
       </c>
       <c r="B10" s="3">
-        <v>0.61902781602500001</v>
+        <v>0.560535090683</v>
       </c>
       <c r="C10" s="3">
-        <v>0.21274520740700001</v>
+        <v>0.151824036399</v>
       </c>
       <c r="D10" s="3">
-        <v>0.141840668753</v>
+        <v>6.0283885746599999E-2</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -2630,13 +2628,13 @@
         <v>10</v>
       </c>
       <c r="B11" s="3">
-        <v>0.61310005560500003</v>
+        <v>0.54889145580700005</v>
       </c>
       <c r="C11" s="3">
-        <v>0.192089435808</v>
+        <v>0.14410997401199999</v>
       </c>
       <c r="D11" s="3">
-        <v>0.14195119304699999</v>
+        <v>5.8538086400699997E-2</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -2644,13 +2642,13 @@
         <v>11</v>
       </c>
       <c r="B12" s="3">
-        <v>0.60682556511499997</v>
+        <v>0.53760175463000004</v>
       </c>
       <c r="C12" s="3">
-        <v>0.17975253370899999</v>
+        <v>0.137045335687</v>
       </c>
       <c r="D12" s="3">
-        <v>0.14270036089400001</v>
+        <v>5.5965265165999999E-2</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -2658,13 +2656,13 @@
         <v>12</v>
       </c>
       <c r="B13" s="3">
-        <v>0.60003715774499999</v>
+        <v>0.52684775526200001</v>
       </c>
       <c r="C13" s="3">
-        <v>0.16576294932300001</v>
+        <v>0.12794835822699999</v>
       </c>
       <c r="D13" s="3">
-        <v>0.14308701596199999</v>
+        <v>5.4510837537599999E-2</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -2672,13 +2670,13 @@
         <v>13</v>
       </c>
       <c r="B14" s="3">
-        <v>0.59258562706399998</v>
+        <v>0.51675156369999997</v>
       </c>
       <c r="C14" s="3">
-        <v>0.152560898449</v>
+        <v>0.116373542883</v>
       </c>
       <c r="D14" s="3">
-        <v>0.143103312402</v>
+        <v>5.3124856982999999E-2</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -2686,13 +2684,13 @@
         <v>14</v>
       </c>
       <c r="B15" s="3">
-        <v>0.584342978869</v>
+        <v>0.50736022685100002</v>
       </c>
       <c r="C15" s="3">
-        <v>0.14276450164900001</v>
+        <v>0.11129558170000001</v>
       </c>
       <c r="D15" s="3">
-        <v>0.141834824271</v>
+        <v>5.2068626769899998E-2</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -2700,13 +2698,13 @@
         <v>15</v>
       </c>
       <c r="B16" s="3">
-        <v>0.57520928755599998</v>
+        <v>0.498654893032</v>
       </c>
       <c r="C16" s="3">
-        <v>0.13722178140999999</v>
+        <v>0.106973366206</v>
       </c>
       <c r="D16" s="3">
-        <v>0.13259396091600001</v>
+        <v>5.1093446985199999E-2</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -2714,13 +2712,13 @@
         <v>16</v>
       </c>
       <c r="B17" s="3">
-        <v>0.56512249692399996</v>
+        <v>0.49057341268499999</v>
       </c>
       <c r="C17" s="3">
-        <v>0.13414221787300001</v>
+        <v>0.101503148852</v>
       </c>
       <c r="D17" s="3">
-        <v>0.12219337072</v>
+        <v>5.0248456620700002E-2</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -2728,13 +2726,13 @@
         <v>17</v>
       </c>
       <c r="B18" s="3">
-        <v>0.55406936086299996</v>
+        <v>0.48303302948499999</v>
       </c>
       <c r="C18" s="3">
-        <v>0.13182593228700001</v>
+        <v>9.5964512714600006E-2</v>
       </c>
       <c r="D18" s="3">
-        <v>0.107234478429</v>
+        <v>4.9479246746299999E-2</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -2742,13 +2740,13 @@
         <v>18</v>
       </c>
       <c r="B19" s="3">
-        <v>0.54209491010800004</v>
+        <v>0.47594690035999998</v>
       </c>
       <c r="C19" s="3">
-        <v>0.130199707548</v>
+        <v>9.1750288430099997E-2</v>
       </c>
       <c r="D19" s="3">
-        <v>0.100113052467</v>
+        <v>4.8692161844E-2</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -2756,13 +2754,13 @@
         <v>19</v>
       </c>
       <c r="B20" s="3">
-        <v>0.52930736796800004</v>
+        <v>0.46923411956099997</v>
       </c>
       <c r="C20" s="3">
-        <v>0.12867145468899999</v>
+        <v>8.8718132032400004E-2</v>
       </c>
       <c r="D20" s="3">
-        <v>9.01149922825E-2</v>
+        <v>4.7755079942799997E-2</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -2770,13 +2768,13 @@
         <v>20</v>
       </c>
       <c r="B21" s="3">
-        <v>0.51587564524200002</v>
+        <v>0.46282524002600001</v>
       </c>
       <c r="C21" s="3">
-        <v>0.12720769858</v>
+        <v>8.6073629473699995E-2</v>
       </c>
       <c r="D21" s="3">
-        <v>7.4069564636899995E-2</v>
+        <v>4.7242679311700002E-2</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -2784,13 +2782,13 @@
         <v>21</v>
       </c>
       <c r="B22" s="3">
-        <v>0.50201775212800004</v>
+        <v>0.45666542110699998</v>
       </c>
       <c r="C22" s="3">
-        <v>0.12561678097500001</v>
+        <v>8.3462615947600002E-2</v>
       </c>
       <c r="D22" s="3">
-        <v>6.4198415500899997E-2</v>
+        <v>4.6899102053100002E-2</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -2798,13 +2796,13 @@
         <v>22</v>
       </c>
       <c r="B23" s="3">
-        <v>0.48798074040900002</v>
+        <v>0.45071668720500002</v>
       </c>
       <c r="C23" s="3">
-        <v>0.123823669104</v>
+        <v>8.0729818398299999E-2</v>
       </c>
       <c r="D23" s="3">
-        <v>5.9101535604900002E-2</v>
+        <v>4.6530683822700002E-2</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -2812,13 +2810,13 @@
         <v>23</v>
       </c>
       <c r="B24" s="3">
-        <v>0.474015572685</v>
+        <v>0.44495992233300002</v>
       </c>
       <c r="C24" s="3">
-        <v>0.121799617458</v>
+        <v>7.7802491255200001E-2</v>
       </c>
       <c r="D24" s="3">
-        <v>5.64756064452E-2</v>
+        <v>4.6138414098100003E-2</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -2826,13 +2824,13 @@
         <v>24</v>
       </c>
       <c r="B25" s="3">
-        <v>0.46035233357900002</v>
+        <v>0.43939630430900001</v>
       </c>
       <c r="C25" s="3">
-        <v>0.119660607658</v>
+        <v>7.4679692994100003E-2</v>
       </c>
       <c r="D25" s="3">
-        <v>5.3690001017599999E-2</v>
+        <v>4.3996111176400003E-2</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -2840,13 +2838,13 @@
         <v>25</v>
       </c>
       <c r="B26" s="3">
-        <v>0.44718119091500003</v>
+        <v>0.43404705194999998</v>
       </c>
       <c r="C26" s="3">
-        <v>0.117595314943</v>
+        <v>7.1398980069599993E-2</v>
       </c>
       <c r="D26" s="3">
-        <v>5.19292441031E-2</v>
+        <v>4.3475248324299998E-2</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -2854,13 +2852,13 @@
         <v>26</v>
       </c>
       <c r="B27" s="3">
-        <v>0.43464234108499999</v>
+        <v>0.42894994915899998</v>
       </c>
       <c r="C27" s="3">
-        <v>0.11559621434</v>
+        <v>6.7959761025399995E-2</v>
       </c>
       <c r="D27" s="3">
-        <v>5.09234287737E-2</v>
+        <v>4.3523584376500002E-2</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -2868,13 +2866,13 @@
         <v>27</v>
       </c>
       <c r="B28" s="3">
-        <v>0.42282505152200001</v>
+        <v>0.42415160992399997</v>
       </c>
       <c r="C28" s="3">
-        <v>0.11358939204100001</v>
+        <v>6.4301805693799993E-2</v>
       </c>
       <c r="D28" s="3">
-        <v>5.0373168388200003E-2</v>
+        <v>4.3074911228899997E-2</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -2882,13 +2880,13 @@
         <v>28</v>
       </c>
       <c r="B29" s="3">
-        <v>0.41177345467600002</v>
+        <v>0.41969622508299997</v>
       </c>
       <c r="C29" s="3">
-        <v>0.111595804634</v>
+        <v>6.0288487501500003E-2</v>
       </c>
       <c r="D29" s="3">
-        <v>4.9753958882099998E-2</v>
+        <v>4.2882167797599999E-2</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -2896,13 +2894,13 @@
         <v>29</v>
       </c>
       <c r="B30" s="3">
-        <v>0.401495817561</v>
+        <v>0.41561398603499999</v>
       </c>
       <c r="C30" s="3">
-        <v>0.109647471545</v>
+        <v>5.5914613666500003E-2</v>
       </c>
       <c r="D30" s="3">
-        <v>4.9203150638200001E-2</v>
+        <v>4.2695712945900001E-2</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -2910,13 +2908,13 @@
         <v>30</v>
       </c>
       <c r="B31" s="3">
-        <v>0.39197443891700001</v>
+        <v>0.41191344662599999</v>
       </c>
       <c r="C31" s="3">
-        <v>0.107754579287</v>
+        <v>5.1450614983999998E-2</v>
       </c>
       <c r="D31" s="3">
-        <v>4.8543402866799999E-2</v>
+        <v>4.2620310498199997E-2</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -2924,13 +2922,13 @@
         <v>31</v>
       </c>
       <c r="B32" s="3">
-        <v>0.38317439705</v>
+        <v>0.40858016935399999</v>
       </c>
       <c r="C32" s="3">
-        <v>0.105922650942</v>
+        <v>4.70943851161E-2</v>
       </c>
       <c r="D32" s="3">
-        <v>4.81220011229E-2</v>
+        <v>4.25925449754E-2</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -2938,13 +2936,13 @@
         <v>32</v>
       </c>
       <c r="B33" s="3">
-        <v>0.37505042611700001</v>
+        <v>0.40558056625799999</v>
       </c>
       <c r="C33" s="3">
-        <v>0.10414955767300001</v>
+        <v>4.28695964193E-2</v>
       </c>
       <c r="D33" s="3">
-        <v>4.7863176803900002E-2</v>
+        <v>4.2601950229199999E-2</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -2952,13 +2950,13 @@
         <v>33</v>
       </c>
       <c r="B34" s="3">
-        <v>0.36755191067100002</v>
+        <v>0.402867914868</v>
       </c>
       <c r="C34" s="3">
-        <v>0.10241697924</v>
+        <v>3.8857454205000003E-2</v>
       </c>
       <c r="D34" s="3">
-        <v>4.7640836945099997E-2</v>
+        <v>4.25672831574E-2</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -2966,13 +2964,13 @@
         <v>34</v>
       </c>
       <c r="B35" s="3">
-        <v>0.36062632758300001</v>
+        <v>0.400388029541</v>
       </c>
       <c r="C35" s="3">
-        <v>0.10069378842899999</v>
+        <v>3.5127290172400003E-2</v>
       </c>
       <c r="D35" s="3">
-        <v>4.7519556104299997E-2</v>
+        <v>4.2650869346999999E-2</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
@@ -2980,13 +2978,13 @@
         <v>35</v>
       </c>
       <c r="B36" s="3">
-        <v>0.35422154198299999</v>
+        <v>0.39808359997100001</v>
       </c>
       <c r="C36" s="3">
-        <v>9.8943523955699997E-2</v>
+        <v>3.1818789877E-2</v>
       </c>
       <c r="D36" s="3">
-        <v>4.7463555423700003E-2</v>
+        <v>4.2425738542100001E-2</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
@@ -2994,13 +2992,13 @@
         <v>36</v>
       </c>
       <c r="B37" s="3">
-        <v>0.34828730770499999</v>
+        <v>0.39589736257500002</v>
       </c>
       <c r="C37" s="3">
-        <v>9.7126047424600001E-2</v>
+        <v>2.90424844067E-2</v>
       </c>
       <c r="D37" s="3">
-        <v>4.7460679022799997E-2</v>
+        <v>4.2540524281100001E-2</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
@@ -3008,13 +3006,13 @@
         <v>37</v>
       </c>
       <c r="B38" s="3">
-        <v>0.34277622508</v>
+        <v>0.39377466878</v>
       </c>
       <c r="C38" s="3">
-        <v>9.5193099818800003E-2</v>
+        <v>2.6859754262300001E-2</v>
       </c>
       <c r="D38" s="3">
-        <v>4.7501966045299999E-2</v>
+        <v>4.2772117213500001E-2</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
@@ -3022,13 +3020,13 @@
         <v>38</v>
       </c>
       <c r="B39" s="3">
-        <v>0.33764432009299999</v>
+        <v>0.3916658905</v>
       </c>
       <c r="C39" s="3">
-        <v>9.3082629322600002E-2</v>
+        <v>2.5217640154399999E-2</v>
       </c>
       <c r="D39" s="3">
-        <v>4.7584196629500003E-2</v>
+        <v>4.2810427904300001E-2</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
@@ -3036,13 +3034,13 @@
         <v>39</v>
       </c>
       <c r="B40" s="3">
-        <v>0.33285134729299998</v>
+        <v>0.38952879157800002</v>
       </c>
       <c r="C40" s="3">
-        <v>9.0717056656200001E-2</v>
+        <v>2.4015571732700001E-2</v>
       </c>
       <c r="D40" s="3">
-        <v>4.76953547327E-2</v>
+        <v>4.3084639327300001E-2</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
@@ -3050,13 +3048,13 @@
         <v>40</v>
       </c>
       <c r="B41" s="3">
-        <v>0.32836088402500002</v>
+        <v>0.38733076625599999</v>
       </c>
       <c r="C41" s="3">
-        <v>8.8010692277999999E-2</v>
+        <v>2.3169240174599998E-2</v>
       </c>
       <c r="D41" s="3">
-        <v>4.7795787405199998E-2</v>
+        <v>4.3244048616699997E-2</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
@@ -3064,13 +3062,13 @@
         <v>41</v>
       </c>
       <c r="B42" s="3">
-        <v>0.32414026699999998</v>
+        <v>0.38505090367099998</v>
       </c>
       <c r="C42" s="3">
-        <v>8.4883776039000006E-2</v>
+        <v>2.2593303725599999E-2</v>
       </c>
       <c r="D42" s="3">
-        <v>4.7814139870299997E-2</v>
+        <v>4.3454181567400003E-2</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
@@ -3078,13 +3076,13 @@
         <v>42</v>
       </c>
       <c r="B43" s="3">
-        <v>0.32016041454700001</v>
+        <v>0.38268221730700003</v>
       </c>
       <c r="C43" s="3">
-        <v>8.1247012098599997E-2</v>
+        <v>2.2205401376600001E-2</v>
       </c>
       <c r="D43" s="3">
-        <v>4.7848748347400001E-2</v>
+        <v>4.3692220748300002E-2</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
@@ -3092,13 +3090,13 @@
         <v>43</v>
       </c>
       <c r="B44" s="3">
-        <v>0.31639557288100001</v>
+        <v>0.38023469558599998</v>
       </c>
       <c r="C44" s="3">
-        <v>7.6918161240000005E-2</v>
+        <v>2.1941625630699998E-2</v>
       </c>
       <c r="D44" s="3">
-        <v>4.78945102053E-2</v>
+        <v>4.39600148658E-2</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
@@ -3106,13 +3104,13 @@
         <v>44</v>
       </c>
       <c r="B45" s="3">
-        <v>0.31282301921599998</v>
+        <v>0.37773921159200002</v>
       </c>
       <c r="C45" s="3">
-        <v>7.1605799203100007E-2</v>
+        <v>2.1759903959500001E-2</v>
       </c>
       <c r="D45" s="3">
-        <v>4.7954160287200003E-2</v>
+        <v>4.4245495465100003E-2</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
@@ -3120,13 +3118,13 @@
         <v>45</v>
       </c>
       <c r="B46" s="3">
-        <v>0.30942274818999999</v>
+        <v>0.37525023906600002</v>
       </c>
       <c r="C46" s="3">
-        <v>6.5204150287799995E-2</v>
+        <v>2.1634265235200002E-2</v>
       </c>
       <c r="D46" s="3">
-        <v>4.8023220426300001E-2</v>
+        <v>4.4649663821299999E-2</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
@@ -3134,13 +3132,13 @@
         <v>46</v>
       </c>
       <c r="B47" s="3">
-        <v>0.306177161197</v>
+        <v>0.37284313636499999</v>
       </c>
       <c r="C47" s="3">
-        <v>5.7874361433600002E-2</v>
+        <v>2.1548457814799998E-2</v>
       </c>
       <c r="D47" s="3">
-        <v>4.81002348336E-2</v>
+        <v>4.4959466251800001E-2</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
@@ -3148,13 +3146,13 @@
         <v>47</v>
       </c>
       <c r="B48" s="3">
-        <v>0.30307077191800003</v>
+        <v>0.37060274704899998</v>
       </c>
       <c r="C48" s="3">
-        <v>4.9593286397200002E-2</v>
+        <v>2.1491815836199999E-2</v>
       </c>
       <c r="D48" s="3">
-        <v>4.81837747353E-2</v>
+        <v>4.6418392431400002E-2</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
@@ -3162,13 +3160,13 @@
         <v>48</v>
       </c>
       <c r="B49" s="3">
-        <v>0.30008993591100003</v>
+        <v>0.36860550058500002</v>
       </c>
       <c r="C49" s="3">
-        <v>4.1165995102499998E-2</v>
+        <v>2.14569952578E-2</v>
       </c>
       <c r="D49" s="3">
-        <v>4.8272751324099999E-2</v>
+        <v>4.6288951984000001E-2</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
@@ -3176,13 +3174,13 @@
         <v>49</v>
       </c>
       <c r="B50" s="3">
-        <v>0.29722260804900003</v>
+        <v>0.36690274290699998</v>
       </c>
       <c r="C50" s="3">
-        <v>3.4467093487500003E-2</v>
+        <v>2.1438749524999998E-2</v>
       </c>
       <c r="D50" s="3">
-        <v>4.8369052414400003E-2</v>
+        <v>4.6588506521699997E-2</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
@@ -3190,13 +3188,13 @@
         <v>50</v>
       </c>
       <c r="B51" s="3">
-        <v>0.294458128619</v>
+        <v>0.36551283828100001</v>
       </c>
       <c r="C51" s="3">
-        <v>3.0005858591099999E-2</v>
+        <v>2.14332278582E-2</v>
       </c>
       <c r="D51" s="3">
-        <v>4.8470281059600002E-2</v>
+        <v>4.6297848248500001E-2</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
@@ -3204,13 +3202,13 @@
         <v>51</v>
       </c>
       <c r="B52" s="3">
-        <v>0.29178703707999998</v>
+        <v>0.36442389196000002</v>
       </c>
       <c r="C52" s="3">
-        <v>2.7038464221400001E-2</v>
+        <v>2.14375443265E-2</v>
       </c>
       <c r="D52" s="3">
-        <v>4.8575322621100002E-2</v>
+        <v>4.5864488155099997E-2</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
@@ -3218,13 +3216,13 @@
         <v>52</v>
       </c>
       <c r="B53" s="3">
-        <v>0.28920091132300002</v>
+        <v>0.36360332662599998</v>
       </c>
       <c r="C53" s="3">
-        <v>2.4973953981499999E-2</v>
+        <v>2.1449498881E-2</v>
       </c>
       <c r="D53" s="3">
-        <v>4.86835134847E-2</v>
+        <v>4.5556539480700001E-2</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
@@ -3232,13 +3230,13 @@
         <v>53</v>
       </c>
       <c r="B54" s="3">
-        <v>0.28669222982300002</v>
+        <v>0.36300889088600002</v>
       </c>
       <c r="C54" s="3">
-        <v>2.3571324211399999E-2</v>
+        <v>2.14673902336E-2</v>
       </c>
       <c r="D54" s="3">
-        <v>4.8794398427999999E-2</v>
+        <v>4.4384468582100003E-2</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
@@ -3246,13 +3244,13 @@
         <v>54</v>
       </c>
       <c r="B55" s="3">
-        <v>0.28425425386399999</v>
+        <v>0.362597361359</v>
       </c>
       <c r="C55" s="3">
-        <v>2.26397190336E-2</v>
+        <v>2.1489887111999999E-2</v>
       </c>
       <c r="D55" s="3">
-        <v>4.8907948989999998E-2</v>
+        <v>4.3796630452400002E-2</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
@@ -3260,13 +3258,13 @@
         <v>55</v>
       </c>
       <c r="B56" s="3">
-        <v>0.28188092716000002</v>
+        <v>0.36232970639099998</v>
       </c>
       <c r="C56" s="3">
-        <v>2.2017737006500001E-2</v>
+        <v>2.1515937786799999E-2</v>
       </c>
       <c r="D56" s="3">
-        <v>4.90239045453E-2</v>
+        <v>4.2981783443799999E-2</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
@@ -3274,13 +3272,13 @@
         <v>56</v>
       </c>
       <c r="B57" s="3">
-        <v>0.27956679035699999</v>
+        <v>0.36217316897700003</v>
       </c>
       <c r="C57" s="3">
-        <v>2.1596370221299999E-2</v>
+        <v>2.1544705219699999E-2</v>
       </c>
       <c r="D57" s="3">
-        <v>4.9142004133699999E-2</v>
+        <v>4.3063526743799999E-2</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
@@ -3288,13 +3286,13 @@
         <v>57</v>
       </c>
       <c r="B58" s="3">
-        <v>0.27730690822600002</v>
+        <v>0.36210134279299999</v>
       </c>
       <c r="C58" s="3">
-        <v>2.1310446786300001E-2</v>
+        <v>2.1575519661399999E-2</v>
       </c>
       <c r="D58" s="3">
-        <v>4.9262170637600002E-2</v>
+        <v>4.3533137537300003E-2</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
@@ -3302,13 +3300,13 @@
         <v>58</v>
       </c>
       <c r="B59" s="3">
-        <v>0.27509680757900001</v>
+        <v>0.362093260473</v>
       </c>
       <c r="C59" s="3">
-        <v>2.1120581327900002E-2</v>
+        <v>2.1607843327700001E-2</v>
       </c>
       <c r="D59" s="3">
-        <v>4.9384254518900002E-2</v>
+        <v>4.3921066230500003E-2</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
@@ -3316,13 +3314,13 @@
         <v>59</v>
       </c>
       <c r="B60" s="3">
-        <v>0.27293242428999998</v>
+        <v>0.36213220678800001</v>
       </c>
       <c r="C60" s="3">
-        <v>2.10011047757E-2</v>
+        <v>2.1641243584600001E-2</v>
       </c>
       <c r="D60" s="3">
-        <v>4.9507929431399998E-2</v>
+        <v>4.38532449757E-2</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
@@ -3330,13 +3328,13 @@
         <v>60</v>
       </c>
       <c r="B61" s="3">
-        <v>0.27081005798699997</v>
+        <v>0.36220464695600002</v>
       </c>
       <c r="C61" s="3">
-        <v>2.0934099386999999E-2</v>
+        <v>2.1675372240200001E-2</v>
       </c>
       <c r="D61" s="3">
-        <v>4.9633062866399999E-2</v>
+        <v>4.3982965858600002E-2</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
@@ -3344,13 +3342,13 @@
         <v>61</v>
       </c>
       <c r="B62" s="3">
-        <v>0.26872633324599998</v>
+        <v>0.362299413919</v>
       </c>
       <c r="C62" s="3">
-        <v>2.0906535477499998E-2</v>
+        <v>2.1709949307200001E-2</v>
       </c>
       <c r="D62" s="3">
-        <v>4.9759441393499998E-2</v>
+        <v>4.4282772808900001E-2</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
@@ -3358,13 +3356,13 @@
         <v>62</v>
       </c>
       <c r="B63" s="3">
-        <v>0.26667816629300001</v>
+        <v>0.36240714992799999</v>
       </c>
       <c r="C63" s="3">
-        <v>2.0908724349299999E-2</v>
+        <v>2.1744750105800001E-2</v>
       </c>
       <c r="D63" s="3">
-        <v>4.98874692983E-2</v>
+        <v>4.4571298768300002E-2</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
@@ -3372,13 +3370,13 @@
         <v>63</v>
       </c>
       <c r="B64" s="3">
-        <v>0.26466273638299997</v>
+        <v>0.36251993618700001</v>
       </c>
       <c r="C64" s="3">
-        <v>2.09333618808E-2</v>
+        <v>2.1779594913200001E-2</v>
       </c>
       <c r="D64" s="3">
-        <v>5.0018070377300002E-2</v>
+        <v>4.51914881905E-2</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
@@ -3386,13 +3384,13 @@
         <v>64</v>
       </c>
       <c r="B65" s="3">
-        <v>0.26267746115500001</v>
+        <v>0.36263104185799999</v>
       </c>
       <c r="C65" s="3">
-        <v>2.0974885914799998E-2</v>
+        <v>2.18143405912E-2</v>
       </c>
       <c r="D65" s="3">
-        <v>5.0150660637499997E-2</v>
+        <v>4.5990516251099997E-2</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
@@ -3400,13 +3398,13 @@
         <v>65</v>
       </c>
       <c r="B66" s="3">
-        <v>0.26071997537500002</v>
+        <v>0.36273474814399997</v>
       </c>
       <c r="C66" s="3">
-        <v>2.10290264754E-2</v>
+        <v>2.1848873776200001E-2</v>
       </c>
       <c r="D66" s="3">
-        <v>5.0284370980999998E-2</v>
+        <v>4.7840880006299998E-2</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
@@ -3414,13 +3412,13 @@
         <v>66</v>
       </c>
       <c r="B67" s="3">
-        <v>0.25878811257200002</v>
+        <v>0.36282622922300001</v>
       </c>
       <c r="C67" s="3">
-        <v>2.1092484072300001E-2</v>
+        <v>2.18831053214E-2</v>
       </c>
       <c r="D67" s="3">
-        <v>5.0419133466E-2</v>
+        <v>5.3609877573699997E-2</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
@@ -3428,13 +3426,13 @@
         <v>67</v>
       </c>
       <c r="B68" s="3">
-        <v>0.25687988912999998</v>
+        <v>0.362901486941</v>
       </c>
       <c r="C68" s="3">
-        <v>2.1162696145999998E-2</v>
+        <v>2.1916965751900001E-2</v>
       </c>
       <c r="D68" s="3">
-        <v>5.05549354829E-2</v>
+        <v>5.1632260236699999E-2</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
@@ -3442,13 +3440,13 @@
         <v>68</v>
       </c>
       <c r="B69" s="3">
-        <v>0.25499349049499997</v>
+        <v>0.36295733822300003</v>
       </c>
       <c r="C69" s="3">
-        <v>2.1237665285300002E-2</v>
+        <v>2.1950401547600001E-2</v>
       </c>
       <c r="D69" s="3">
-        <v>5.0691777952E-2</v>
+        <v>5.6203491671999999E-2</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
@@ -3456,13 +3454,13 @@
         <v>69</v>
       </c>
       <c r="B70" s="3">
-        <v>0.25312725915399997</v>
+        <v>0.36299144724999999</v>
       </c>
       <c r="C70" s="3">
-        <v>2.13158313143E-2</v>
+        <v>2.19833721047E-2</v>
       </c>
       <c r="D70" s="3">
-        <v>5.0829666856899998E-2</v>
+        <v>5.85175214463E-2</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
@@ -3470,13 +3468,13 @@
         <v>70</v>
       </c>
       <c r="B71" s="3">
-        <v>0.251279684133</v>
+        <v>0.36300238419800002</v>
       </c>
       <c r="C71" s="3">
-        <v>2.1395974911399999E-2</v>
+        <v>2.2015847255700001E-2</v>
       </c>
       <c r="D71" s="3">
-        <v>5.0968611202199997E-2</v>
+        <v>5.6247856064100002E-2</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
@@ -3484,13 +3482,13 @@
         <v>71</v>
       </c>
       <c r="B72" s="3">
-        <v>0.24944939177100001</v>
+        <v>0.36298968409100002</v>
       </c>
       <c r="C72" s="3">
-        <v>2.14771441706E-2</v>
+        <v>2.2047805249100001E-2</v>
       </c>
       <c r="D72" s="3">
-        <v>5.11086222681E-2</v>
+        <v>5.1976224754000003E-2</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
@@ -3498,13 +3496,13 @@
         <v>72</v>
       </c>
       <c r="B73" s="3">
-        <v>0.247635137556</v>
+        <v>0.36295387695199999</v>
       </c>
       <c r="C73" s="3">
-        <v>2.1558598066099999E-2</v>
+        <v>2.20792311074E-2</v>
       </c>
       <c r="D73" s="3">
-        <v>5.1249713139299997E-2</v>
+        <v>4.8662203624199998E-2</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
@@ -3512,13 +3510,13 @@
         <v>73</v>
       </c>
       <c r="B74" s="3">
-        <v>0.245835798844</v>
+        <v>0.362896465532</v>
       </c>
       <c r="C74" s="3">
-        <v>2.16397625265E-2</v>
+        <v>2.2110115296600001E-2</v>
       </c>
       <c r="D74" s="3">
-        <v>5.1391898321800002E-2</v>
+        <v>4.4849812917199999E-2</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
@@ -3526,13 +3524,13 @@
         <v>74</v>
       </c>
       <c r="B75" s="3">
-        <v>0.24405036830599999</v>
+        <v>0.362819838512</v>
       </c>
       <c r="C75" s="3">
-        <v>2.17201960322E-2</v>
+        <v>2.21404526499E-2</v>
       </c>
       <c r="D75" s="3">
-        <v>5.1535193407800002E-2</v>
+        <v>4.3098904660100003E-2</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
@@ -3540,13 +3538,13 @@
         <v>75</v>
       </c>
       <c r="B76" s="3">
-        <v>0.24227794795099999</v>
+        <v>0.362727121815</v>
       </c>
       <c r="C76" s="3">
-        <v>2.1799562488799998E-2</v>
+        <v>2.2170241500399999E-2</v>
       </c>
       <c r="D76" s="3">
-        <v>5.16796147727E-2</v>
+        <v>4.0137199697599997E-2</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
@@ -3554,13 +3552,13 @@
         <v>76</v>
       </c>
       <c r="B77" s="3">
-        <v>0.24051774361100001</v>
+        <v>0.36262198406399998</v>
       </c>
       <c r="C77" s="3">
-        <v>2.1877609720799999E-2</v>
+        <v>2.21994829835E-2</v>
       </c>
       <c r="D77" s="3">
-        <v>5.1822394371699998E-2</v>
+        <v>3.6432823618499997E-2</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
@@ -3568,13 +3566,13 @@
         <v>77</v>
       </c>
       <c r="B78" s="3">
-        <v>0.238769059783</v>
+        <v>0.36250842038199999</v>
       </c>
       <c r="C78" s="3">
-        <v>2.1954152345800001E-2</v>
+        <v>2.2228180477700001E-2</v>
       </c>
       <c r="D78" s="3">
-        <v>5.1967988956099997E-2</v>
+        <v>3.3997328561899999E-2</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
@@ -3582,13 +3580,13 @@
         <v>78</v>
       </c>
       <c r="B79" s="3">
-        <v>0.23703129472500001</v>
+        <v>0.36239054000400001</v>
       </c>
       <c r="C79" s="3">
-        <v>2.20290580935E-2</v>
+        <v>2.2256339157399999E-2</v>
       </c>
       <c r="D79" s="3">
-        <v>5.2115461104999997E-2</v>
+        <v>3.3093329802100002E-2</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
@@ -3596,13 +3594,13 @@
         <v>79</v>
       </c>
       <c r="B80" s="3">
-        <v>0.235303935746</v>
+        <v>0.36227237825300002</v>
       </c>
       <c r="C80" s="3">
-        <v>2.2102236849799999E-2</v>
+        <v>2.2283965636099998E-2</v>
       </c>
       <c r="D80" s="3">
-        <v>5.2264399814699998E-2</v>
+        <v>3.0939244933300001E-2</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
@@ -3610,13 +3608,13 @@
         <v>80</v>
       </c>
       <c r="B81" s="3">
-        <v>0.233586554606</v>
+        <v>0.36215774507499998</v>
       </c>
       <c r="C81" s="3">
-        <v>2.2173631870100002E-2</v>
+        <v>2.2311067683100001E-2</v>
       </c>
       <c r="D81" s="3">
-        <v>5.2414885129900002E-2</v>
+        <v>3.0386018166399999E-2</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
@@ -3624,13 +3622,13 @@
         <v>81</v>
       </c>
       <c r="B82" s="3">
-        <v>0.23187880298300001</v>
+        <v>0.362050113349</v>
       </c>
       <c r="C82" s="3">
-        <v>2.2243212726100001E-2</v>
+        <v>2.2337653998100001E-2</v>
       </c>
       <c r="D82" s="3">
-        <v>5.25668706024E-2</v>
+        <v>2.9868952767399998E-2</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
@@ -3638,13 +3636,13 @@
         <v>82</v>
       </c>
       <c r="B83" s="3">
-        <v>0.23018040796799999</v>
+        <v>0.361952542923</v>
       </c>
       <c r="C83" s="3">
-        <v>2.2310969641199999E-2</v>
+        <v>2.2363734033300001E-2</v>
       </c>
       <c r="D83" s="3">
-        <v>5.27203497735E-2</v>
+        <v>2.8729823774200001E-2</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
@@ -3652,13 +3650,13 @@
         <v>83</v>
       </c>
       <c r="B84" s="3">
-        <v>0.22849116753900001</v>
+        <v>0.36186763186100002</v>
       </c>
       <c r="C84" s="3">
-        <v>2.2376908942E-2</v>
+        <v>2.2389317851800001E-2</v>
       </c>
       <c r="D84" s="3">
-        <v>5.2875320461500001E-2</v>
+        <v>2.8339435015100001E-2</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
@@ -3666,13 +3664,13 @@
         <v>84</v>
       </c>
       <c r="B85" s="3">
-        <v>0.22681094600500001</v>
+        <v>0.36179748461599998</v>
       </c>
       <c r="C85" s="3">
-        <v>2.2441049407200001E-2</v>
+        <v>2.2414416017000002E-2</v>
       </c>
       <c r="D85" s="3">
-        <v>5.3028388429100001E-2</v>
+        <v>2.81387112901E-2</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
@@ -3680,13 +3678,13 @@
         <v>85</v>
       </c>
       <c r="B86" s="3">
-        <v>0.22513966939800001</v>
+        <v>0.36174368733099999</v>
       </c>
       <c r="C86" s="3">
-        <v>2.2503419339600001E-2</v>
+        <v>2.2439039503799999E-2</v>
       </c>
       <c r="D86" s="3">
-        <v>5.3181567957199999E-2</v>
+        <v>2.79099234092E-2</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
@@ -3694,13 +3692,13 @@
         <v>86</v>
       </c>
       <c r="B87" s="3">
-        <v>0.223477320796</v>
+        <v>0.36170728240400002</v>
       </c>
       <c r="C87" s="3">
-        <v>2.2564054219900001E-2</v>
+        <v>2.2463199628800001E-2</v>
       </c>
       <c r="D87" s="3">
-        <v>5.3336140089700002E-2</v>
+        <v>2.7885086546300002E-2</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
@@ -3708,13 +3706,13 @@
         <v>87</v>
       </c>
       <c r="B88" s="3">
-        <v>0.221823935597</v>
+        <v>0.36168873740500002</v>
       </c>
       <c r="C88" s="3">
-        <v>2.26229948296E-2</v>
+        <v>2.24869079943E-2</v>
       </c>
       <c r="D88" s="3">
-        <v>5.3492005073899999E-2</v>
+        <v>2.7746583176200001E-2</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
@@ -3722,13 +3720,13 @@
         <v>88</v>
       </c>
       <c r="B89" s="3">
-        <v>0.220179596723</v>
+        <v>0.36168790719100002</v>
       </c>
       <c r="C89" s="3">
-        <v>2.2680285751799999E-2</v>
+        <v>2.2510176442099999E-2</v>
       </c>
       <c r="D89" s="3">
-        <v>5.3649153715499998E-2</v>
+        <v>2.7706075258599999E-2</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
@@ -3736,13 +3734,13 @@
         <v>89</v>
       </c>
       <c r="B90" s="3">
-        <v>0.21854442977999999</v>
+        <v>0.36170399260800001</v>
       </c>
       <c r="C90" s="3">
-        <v>2.2735974175899999E-2</v>
+        <v>2.2533017016500002E-2</v>
       </c>
       <c r="D90" s="3">
-        <v>5.3807600006499999E-2</v>
+        <v>2.7516317019700001E-2</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
@@ -3750,13 +3748,13 @@
         <v>90</v>
       </c>
       <c r="B91" s="3">
-        <v>0.21691859818199999</v>
+        <v>0.36173550455499998</v>
       </c>
       <c r="C91" s="3">
-        <v>2.2790108947900001E-2</v>
+        <v>2.2555441931600001E-2</v>
       </c>
       <c r="D91" s="3">
-        <v>5.3967354040199998E-2</v>
+        <v>2.7400943541199999E-2</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
@@ -3764,13 +3762,13 @@
         <v>91</v>
       </c>
       <c r="B92" s="3">
-        <v>0.21530229826200001</v>
+        <v>0.36178024801199998</v>
       </c>
       <c r="C92" s="3">
-        <v>2.2842739817599999E-2</v>
+        <v>2.2577463542799998E-2</v>
       </c>
       <c r="D92" s="3">
-        <v>5.4128421151799999E-2</v>
+        <v>2.71895343994E-2</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
@@ -3778,13 +3776,13 @@
         <v>92</v>
       </c>
       <c r="B93" s="3">
-        <v>0.21369575439399999</v>
+        <v>0.36183534563800002</v>
       </c>
       <c r="C93" s="3">
-        <v>2.2893916844900001E-2</v>
+        <v>2.2599094320900001E-2</v>
       </c>
       <c r="D93" s="3">
-        <v>5.42662039161E-2</v>
+        <v>2.7119308096500001E-2</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
@@ -3792,13 +3790,13 @@
         <v>93</v>
       </c>
       <c r="B94" s="3">
-        <v>0.21209921413899999</v>
+        <v>0.36189732230400001</v>
       </c>
       <c r="C94" s="3">
-        <v>2.2943689933499999E-2</v>
+        <v>2.26203468262E-2</v>
       </c>
       <c r="D94" s="3">
-        <v>5.4378228759800001E-2</v>
+        <v>2.6935047878399999E-2</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
@@ -3806,13 +3804,13 @@
         <v>94</v>
       </c>
       <c r="B95" s="3">
-        <v>0.210512943471</v>
+        <v>0.36196226725199998</v>
       </c>
       <c r="C95" s="3">
-        <v>2.29921084683E-2</v>
+        <v>2.26412336837E-2</v>
       </c>
       <c r="D95" s="3">
-        <v>5.4483131708899998E-2</v>
+        <v>2.67823531554E-2</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
@@ -3820,13 +3818,13 @@
         <v>95</v>
       </c>
       <c r="B96" s="3">
-        <v>0.20893722209099999</v>
+        <v>0.36202607693700001</v>
       </c>
       <c r="C96" s="3">
-        <v>2.3039221035100001E-2</v>
+        <v>2.26617675574E-2</v>
       </c>
       <c r="D96" s="3">
-        <v>5.4590277609099999E-2</v>
+        <v>2.6644454832200001E-2</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
@@ -3834,13 +3832,13 @@
         <v>96</v>
       </c>
       <c r="B97" s="3">
-        <v>0.20737233887100001</v>
+        <v>0.36208476022899999</v>
       </c>
       <c r="C97" s="3">
-        <v>2.3085075206600001E-2</v>
+        <v>2.2681961123E-2</v>
       </c>
       <c r="D97" s="3">
-        <v>5.47008582592E-2</v>
+        <v>2.6580612120499999E-2</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
@@ -3848,13 +3846,13 @@
         <v>97</v>
       </c>
       <c r="B98" s="3">
-        <v>0.20581858747599999</v>
+        <v>0.36213476522799998</v>
       </c>
       <c r="C98" s="3">
-        <v>2.3129717382900001E-2</v>
+        <v>2.2701827039200002E-2</v>
       </c>
       <c r="D98" s="3">
-        <v>5.48136230869E-2</v>
+        <v>2.6446171996099999E-2</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
@@ -3862,13 +3860,13 @@
         <v>98</v>
       </c>
       <c r="B99" s="3">
-        <v>0.20427626218</v>
+        <v>0.362173274032</v>
       </c>
       <c r="C99" s="3">
-        <v>2.3173192674E-2</v>
+        <v>2.2721377918E-2</v>
       </c>
       <c r="D99" s="3">
-        <v>5.4928493055100003E-2</v>
+        <v>2.6332486613E-2</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
@@ -3876,13 +3874,13 @@
         <v>99</v>
       </c>
       <c r="B100" s="3">
-        <v>0.20274565392800001</v>
+        <v>0.362198416977</v>
       </c>
       <c r="C100" s="3">
-        <v>2.3215544817999999E-2</v>
+        <v>2.27406262922E-2</v>
       </c>
       <c r="D100" s="3">
-        <v>5.5045523079100003E-2</v>
+        <v>2.6241760678099999E-2</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
@@ -3890,17 +3888,456 @@
         <v>100</v>
       </c>
       <c r="B101" s="3">
-        <v>0.20122704667399999</v>
+        <v>0.36220938022900001</v>
       </c>
       <c r="C101" s="3">
-        <v>2.3256816125899998E-2</v>
+        <v>2.2759584582499999E-2</v>
       </c>
       <c r="D101" s="3">
-        <v>5.5164807540199999E-2</v>
-      </c>
+        <v>2.6326490967300002E-2</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A102" s="1"/>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A103" s="1"/>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A104" s="1"/>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A105" s="1"/>
       <c r="D105" s="2"/>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A106" s="1"/>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A107" s="1"/>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A108" s="1"/>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A109" s="1"/>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A110" s="1"/>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A111" s="1"/>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A112" s="1"/>
+    </row>
+    <row r="113" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A113" s="1"/>
+    </row>
+    <row r="114" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A114" s="1"/>
+    </row>
+    <row r="115" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A115" s="1"/>
+    </row>
+    <row r="116" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A116" s="1"/>
+    </row>
+    <row r="117" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A117" s="1"/>
+    </row>
+    <row r="118" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A118" s="1"/>
+    </row>
+    <row r="119" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A119" s="1"/>
+    </row>
+    <row r="120" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A120" s="1"/>
+    </row>
+    <row r="121" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A121" s="1"/>
+    </row>
+    <row r="122" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A122" s="1"/>
+    </row>
+    <row r="123" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A123" s="1"/>
+    </row>
+    <row r="124" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A124" s="1"/>
+    </row>
+    <row r="125" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A125" s="1"/>
+    </row>
+    <row r="126" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A126" s="1"/>
+    </row>
+    <row r="127" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A127" s="1"/>
+    </row>
+    <row r="128" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A128" s="1"/>
+    </row>
+    <row r="129" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A129" s="1"/>
+    </row>
+    <row r="130" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A130" s="1"/>
+    </row>
+    <row r="131" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A131" s="1"/>
+    </row>
+    <row r="132" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A132" s="1"/>
+    </row>
+    <row r="133" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A133" s="1"/>
+    </row>
+    <row r="134" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A134" s="1"/>
+    </row>
+    <row r="135" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A135" s="1"/>
+    </row>
+    <row r="136" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A136" s="1"/>
+    </row>
+    <row r="137" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A137" s="1"/>
+    </row>
+    <row r="138" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A138" s="1"/>
+    </row>
+    <row r="139" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A139" s="1"/>
+    </row>
+    <row r="140" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A140" s="1"/>
+    </row>
+    <row r="141" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A141" s="1"/>
+    </row>
+    <row r="142" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A142" s="1"/>
+    </row>
+    <row r="143" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A143" s="1"/>
+    </row>
+    <row r="144" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A144" s="1"/>
+    </row>
+    <row r="145" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A145" s="1"/>
+    </row>
+    <row r="146" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A146" s="1"/>
+    </row>
+    <row r="147" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A147" s="1"/>
+    </row>
+    <row r="148" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A148" s="1"/>
+    </row>
+    <row r="149" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A149" s="1"/>
+    </row>
+    <row r="150" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A150" s="1"/>
+    </row>
+    <row r="151" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A151" s="1"/>
+    </row>
+    <row r="152" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A152" s="1"/>
+    </row>
+    <row r="153" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A153" s="1"/>
+    </row>
+    <row r="154" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A154" s="1"/>
+    </row>
+    <row r="155" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A155" s="1"/>
+    </row>
+    <row r="156" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A156" s="1"/>
+    </row>
+    <row r="157" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A157" s="1"/>
+    </row>
+    <row r="158" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A158" s="1"/>
+    </row>
+    <row r="159" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A159" s="1"/>
+    </row>
+    <row r="160" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A160" s="1"/>
+    </row>
+    <row r="161" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A161" s="1"/>
+    </row>
+    <row r="162" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A162" s="1"/>
+    </row>
+    <row r="163" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A163" s="1"/>
+    </row>
+    <row r="164" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A164" s="1"/>
+    </row>
+    <row r="165" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A165" s="1"/>
+    </row>
+    <row r="166" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A166" s="1"/>
+    </row>
+    <row r="167" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A167" s="1"/>
+    </row>
+    <row r="168" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A168" s="1"/>
+    </row>
+    <row r="169" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A169" s="1"/>
+    </row>
+    <row r="170" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A170" s="1"/>
+    </row>
+    <row r="171" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A171" s="1"/>
+    </row>
+    <row r="172" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A172" s="1"/>
+    </row>
+    <row r="173" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A173" s="1"/>
+    </row>
+    <row r="174" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A174" s="1"/>
+    </row>
+    <row r="175" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A175" s="1"/>
+    </row>
+    <row r="176" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A176" s="1"/>
+    </row>
+    <row r="177" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A177" s="1"/>
+    </row>
+    <row r="178" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A178" s="1"/>
+    </row>
+    <row r="179" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A179" s="1"/>
+    </row>
+    <row r="180" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A180" s="1"/>
+    </row>
+    <row r="181" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A181" s="1"/>
+    </row>
+    <row r="182" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A182" s="1"/>
+    </row>
+    <row r="183" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A183" s="1"/>
+    </row>
+    <row r="184" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A184" s="1"/>
+    </row>
+    <row r="185" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A185" s="1"/>
+    </row>
+    <row r="186" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A186" s="1"/>
+    </row>
+    <row r="187" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A187" s="1"/>
+    </row>
+    <row r="188" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A188" s="1"/>
+    </row>
+    <row r="189" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A189" s="1"/>
+    </row>
+    <row r="190" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A190" s="1"/>
+    </row>
+    <row r="191" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A191" s="1"/>
+    </row>
+    <row r="192" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A192" s="1"/>
+    </row>
+    <row r="193" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A193" s="1"/>
+    </row>
+    <row r="194" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A194" s="1"/>
+    </row>
+    <row r="195" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A195" s="1"/>
+    </row>
+    <row r="196" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A196" s="1"/>
+    </row>
+    <row r="197" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A197" s="1"/>
+    </row>
+    <row r="198" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A198" s="1"/>
+    </row>
+    <row r="199" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A199" s="1"/>
+    </row>
+    <row r="200" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A200" s="1"/>
+    </row>
+    <row r="201" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A201" s="1"/>
+    </row>
+    <row r="202" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A202" s="1"/>
+    </row>
+    <row r="203" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A203" s="1"/>
+    </row>
+    <row r="204" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A204" s="1"/>
+    </row>
+    <row r="205" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A205" s="1"/>
+    </row>
+    <row r="206" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A206" s="1"/>
+    </row>
+    <row r="207" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A207" s="1"/>
+    </row>
+    <row r="208" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A208" s="1"/>
+    </row>
+    <row r="209" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A209" s="1"/>
+    </row>
+    <row r="210" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A210" s="1"/>
+    </row>
+    <row r="211" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A211" s="1"/>
+    </row>
+    <row r="212" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A212" s="1"/>
+    </row>
+    <row r="213" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A213" s="1"/>
+    </row>
+    <row r="214" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A214" s="1"/>
+    </row>
+    <row r="215" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A215" s="1"/>
+    </row>
+    <row r="216" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A216" s="1"/>
+    </row>
+    <row r="217" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A217" s="1"/>
+    </row>
+    <row r="218" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A218" s="1"/>
+    </row>
+    <row r="219" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A219" s="1"/>
+    </row>
+    <row r="220" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A220" s="1"/>
+    </row>
+    <row r="221" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A221" s="1"/>
+    </row>
+    <row r="222" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A222" s="1"/>
+    </row>
+    <row r="223" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A223" s="1"/>
+    </row>
+    <row r="224" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A224" s="1"/>
+    </row>
+    <row r="225" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A225" s="1"/>
+    </row>
+    <row r="226" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A226" s="1"/>
+    </row>
+    <row r="227" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A227" s="1"/>
+    </row>
+    <row r="228" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A228" s="1"/>
+    </row>
+    <row r="229" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A229" s="1"/>
+    </row>
+    <row r="230" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A230" s="1"/>
+    </row>
+    <row r="231" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A231" s="1"/>
+    </row>
+    <row r="232" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A232" s="1"/>
+    </row>
+    <row r="233" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A233" s="1"/>
+    </row>
+    <row r="234" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A234" s="1"/>
+    </row>
+    <row r="235" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A235" s="1"/>
+    </row>
+    <row r="236" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A236" s="1"/>
+    </row>
+    <row r="237" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A237" s="1"/>
+    </row>
+    <row r="238" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A238" s="1"/>
+    </row>
+    <row r="239" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A239" s="1"/>
+    </row>
+    <row r="240" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A240" s="1"/>
+    </row>
+    <row r="241" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A241" s="1"/>
+    </row>
+    <row r="242" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A242" s="1"/>
+    </row>
+    <row r="243" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A243" s="1"/>
+    </row>
+    <row r="244" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A244" s="1"/>
+    </row>
+    <row r="245" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A245" s="1"/>
+    </row>
+    <row r="246" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A246" s="1"/>
+    </row>
+    <row r="247" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A247" s="1"/>
+    </row>
+    <row r="248" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A248" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>